<commit_message>
Changed NH3 file name
</commit_message>
<xml_diff>
--- a/data/Figure 1 data.xlsx
+++ b/data/Figure 1 data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au583430_uni_au_dk/Documents/Dokumenter/NH3 from digestate, May 2018 exp/New figure work/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aarhusuniversitet-my.sharepoint.com/personal/au583430_uni_au_dk/Documents/Dokumenter/GitHub/Lemes-2022-digestate-NH3/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{46B97E22-33EE-4E0F-BAB2-5CE47273A738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0B8990F-D473-4DD9-988C-407CB6102624}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{46B97E22-33EE-4E0F-BAB2-5CE47273A738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A593828-59D7-4B8C-BEB0-D70B7C2E8355}"/>
   <bookViews>
-    <workbookView xWindow="-32235" yWindow="-1005" windowWidth="28800" windowHeight="14985" xr2:uid="{96ED7656-DD76-429A-8978-70DFFFB17E68}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{96ED7656-DD76-429A-8978-70DFFFB17E68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -693,11 +693,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4A9DAC-D383-4BED-958E-702B15BB6D81}">
   <dimension ref="A1:D1495"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I280" sqref="I280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>